<commit_message>
models and distribution plots
</commit_message>
<xml_diff>
--- a/RawMaterials/data/LocalAdaptionDataGathering.xlsx
+++ b/RawMaterials/data/LocalAdaptionDataGathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Documents\git\localadaptclim\RawMaterials\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D01B9F8-DA37-4F7E-80A5-03CA7D6D6632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7726FE60-8532-44DB-B566-584C832F57B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="920" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6762" uniqueCount="1204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6767" uniqueCount="1205">
   <si>
     <t>ID1</t>
   </si>
@@ -5139,9 +5139,6 @@
     <t>daily_climate_garden_gathered</t>
   </si>
   <si>
-    <t>missing_prov</t>
-  </si>
-  <si>
     <t>prov46</t>
   </si>
   <si>
@@ -5164,6 +5161,12 @@
   </si>
   <si>
     <t>prov3</t>
+  </si>
+  <si>
+    <t>missing_dailyclim_prov</t>
+  </si>
+  <si>
+    <t>facet_plots_distribution_overlap</t>
   </si>
 </sst>
 </file>
@@ -61047,8 +61050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE38D98-9064-4846-BB7F-8B771A284B01}">
   <dimension ref="A1:T114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -69991,11 +69994,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65599BFC-5B06-4EDE-87C3-57BB3CCD5BDB}">
-  <dimension ref="A1:AG29"/>
+  <dimension ref="A1:AH29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W17" sqref="W17"/>
+      <pane xSplit="2" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -70010,10 +70013,10 @@
     <col min="9" max="9" width="18.09765625" customWidth="1"/>
     <col min="11" max="11" width="21.046875" customWidth="1"/>
     <col min="19" max="19" width="15.6484375" customWidth="1"/>
-    <col min="20" max="24" width="22.796875" customWidth="1"/>
+    <col min="20" max="25" width="22.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.6">
       <c r="B1" s="1" t="s">
         <v>652</v>
       </c>
@@ -70060,7 +70063,7 @@
         <v>1192</v>
       </c>
       <c r="Q1" s="25" t="s">
-        <v>1195</v>
+        <v>1203</v>
       </c>
       <c r="R1" s="25" t="s">
         <v>1194</v>
@@ -70075,19 +70078,22 @@
         <v>970</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>988</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1202</v>
-      </c>
-      <c r="Y1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="Z1" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -70137,7 +70143,7 @@
         <v>672</v>
       </c>
       <c r="Q2" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="R2" t="s">
         <v>672</v>
@@ -70161,7 +70167,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -70209,7 +70215,7 @@
         <v>672</v>
       </c>
       <c r="Q3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="R3" t="s">
         <v>672</v>
@@ -70229,8 +70235,9 @@
       <c r="X3" s="4" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.6">
+      <c r="Y3" s="4"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A19" si="0">A3+1</f>
         <v>3</v>
@@ -70298,18 +70305,19 @@
       <c r="X4" s="10" t="s">
         <v>672</v>
       </c>
-      <c r="Y4" s="46" t="s">
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="46" t="s">
         <v>685</v>
       </c>
-      <c r="Z4" s="46"/>
-      <c r="AB4" t="s">
+      <c r="AA4" s="46"/>
+      <c r="AC4" t="s">
         <v>991</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>1114</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -70357,14 +70365,14 @@
       <c r="U5" t="s">
         <v>695</v>
       </c>
-      <c r="Y5" s="61" t="s">
+      <c r="Z5" s="61" t="s">
         <v>697</v>
       </c>
-      <c r="Z5" s="61"/>
       <c r="AA5" s="61"/>
       <c r="AB5" s="61"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.6">
+      <c r="AC5" s="61"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -70412,7 +70420,7 @@
         <v>672</v>
       </c>
       <c r="Q6" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="R6" s="10" t="s">
         <v>672</v>
@@ -70433,7 +70441,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -70499,7 +70507,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -70565,7 +70573,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -70633,11 +70641,11 @@
       <c r="X9" t="s">
         <v>672</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -70705,11 +70713,11 @@
       <c r="X10" t="s">
         <v>672</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -70757,7 +70765,7 @@
         <v>672</v>
       </c>
       <c r="Q11" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R11" s="61" t="s">
         <v>726</v>
@@ -70771,21 +70779,25 @@
       <c r="U11" t="s">
         <v>695</v>
       </c>
+      <c r="V11" t="s">
+        <v>672</v>
+      </c>
       <c r="W11" t="s">
         <v>695</v>
       </c>
       <c r="X11" s="63"/>
-      <c r="Y11" t="s">
+      <c r="Y11" s="63"/>
+      <c r="Z11" t="s">
         <v>731</v>
       </c>
-      <c r="AF11" s="1" t="s">
+      <c r="AG11" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AH11" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -70850,17 +70862,17 @@
       <c r="X12" t="s">
         <v>672</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>732</v>
       </c>
-      <c r="AF12" s="1" t="s">
+      <c r="AG12" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AH12" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -70922,17 +70934,17 @@
       <c r="X13" t="s">
         <v>672</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>622</v>
       </c>
-      <c r="AF13" s="1" t="s">
+      <c r="AG13" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AH13" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -70997,14 +71009,17 @@
       <c r="X14" t="s">
         <v>672</v>
       </c>
-      <c r="AF14" s="1" t="s">
+      <c r="Y14" t="s">
+        <v>672</v>
+      </c>
+      <c r="AG14" s="1" t="s">
         <v>637</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="AH14" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -71048,17 +71063,17 @@
       <c r="U15" s="62" t="s">
         <v>672</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>887</v>
       </c>
-      <c r="AF15" s="1" t="s">
+      <c r="AG15" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="AH15" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -71123,14 +71138,17 @@
       <c r="X16" t="s">
         <v>672</v>
       </c>
-      <c r="AF16" s="1" t="s">
+      <c r="Y16" t="s">
+        <v>672</v>
+      </c>
+      <c r="AG16" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="AG16" t="s">
+      <c r="AH16" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -71195,14 +71213,14 @@
       <c r="X17" t="s">
         <v>672</v>
       </c>
-      <c r="AF17" s="1" t="s">
+      <c r="AG17" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="AG17" t="s">
+      <c r="AH17" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -71267,23 +71285,23 @@
       <c r="X18" t="s">
         <v>672</v>
       </c>
-      <c r="Y18" s="63" t="s">
-        <v>1201</v>
-      </c>
-      <c r="Z18" s="63"/>
+      <c r="Z18" s="63" t="s">
+        <v>1200</v>
+      </c>
       <c r="AA18" s="63"/>
       <c r="AB18" s="63"/>
       <c r="AC18" s="63"/>
       <c r="AD18" s="63"/>
       <c r="AE18" s="63"/>
-      <c r="AF18" s="1" t="s">
+      <c r="AF18" s="63"/>
+      <c r="AG18" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AH18" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -71331,7 +71349,7 @@
         <v>672</v>
       </c>
       <c r="Q19" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="R19" t="s">
         <v>672</v>
@@ -71351,14 +71369,14 @@
       <c r="X19" t="s">
         <v>672</v>
       </c>
-      <c r="AF19" s="1" t="s">
+      <c r="AG19" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AH19" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A20">
         <v>19</v>
       </c>
@@ -71425,14 +71443,14 @@
       <c r="X20" t="s">
         <v>672</v>
       </c>
-      <c r="AF20" s="1" t="s">
+      <c r="AG20" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="AG20" t="s">
+      <c r="AH20" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A21">
         <f>A20+1</f>
         <v>20</v>
@@ -71500,14 +71518,14 @@
       <c r="X21" t="s">
         <v>672</v>
       </c>
-      <c r="AF21" s="1" t="s">
+      <c r="AG21" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="AG21" t="s">
+      <c r="AH21" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A22">
         <f t="shared" ref="A22:A26" si="1">A21+1</f>
         <v>21</v>
@@ -71575,14 +71593,14 @@
       <c r="X22" t="s">
         <v>672</v>
       </c>
-      <c r="AF22" s="1" t="s">
+      <c r="AG22" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="AG22" t="s">
+      <c r="AH22" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -71620,17 +71638,21 @@
       <c r="L23" t="s">
         <v>1119</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="17" t="s">
         <v>672</v>
       </c>
-      <c r="AF23" s="1" t="s">
+      <c r="N23" t="s">
+        <v>672</v>
+      </c>
+      <c r="R23" s="17"/>
+      <c r="AG23" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="AG23" t="s">
+      <c r="AH23" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -71669,14 +71691,14 @@
       <c r="M24" s="15" t="s">
         <v>1148</v>
       </c>
-      <c r="AF24" s="1" t="s">
+      <c r="AG24" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="AG24" t="s">
+      <c r="AH24" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -71702,14 +71724,14 @@
       <c r="N25" t="s">
         <v>1155</v>
       </c>
-      <c r="AF25" s="1" t="s">
+      <c r="AG25" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="AG25" t="s">
+      <c r="AH25" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.6">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -71753,14 +71775,14 @@
       <c r="N26" t="s">
         <v>1179</v>
       </c>
-      <c r="AF26" s="1" t="s">
+      <c r="AG26" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="AG26" t="s">
+      <c r="AH26" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.6">
       <c r="B27" s="52" t="s">
         <v>1180</v>
       </c>
@@ -71795,7 +71817,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.6">
       <c r="B28" s="10" t="s">
         <v>1187</v>
       </c>
@@ -71833,7 +71855,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.6">
       <c r="B29" s="10" t="s">
         <v>1188</v>
       </c>

</xml_diff>

<commit_message>
ran fall events model, made loop for distribution overlap analysis
</commit_message>
<xml_diff>
--- a/RawMaterials/data/LocalAdaptionDataGathering.xlsx
+++ b/RawMaterials/data/LocalAdaptionDataGathering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Documents\git\localadaptclim\RawMaterials\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7726FE60-8532-44DB-B566-584C832F57B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8310D2F5-23EC-4A47-A0BF-29C12E07A882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="920" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="920" firstSheet="29" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="6" r:id="rId1"/>
@@ -6793,7 +6793,7 @@
   <dimension ref="A1:AB107"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:XFD1048576"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -51928,8 +51928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4ECFFA-8AC8-4048-AA07-B0D2503C1E8B}">
   <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q9:R17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -51968,6 +51968,11 @@
         <v>931</v>
       </c>
     </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.6">
+      <c r="H6">
+        <v>90</v>
+      </c>
+    </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
@@ -52015,7 +52020,7 @@
       <c r="G8" s="12" t="s">
         <v>744</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="21" t="s">
         <v>39</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -52074,8 +52079,8 @@
       <c r="G9" s="4">
         <v>11.116666666666699</v>
       </c>
-      <c r="H9" s="4">
-        <v>27.722000000000001</v>
+      <c r="H9">
+        <v>117.72200000000001</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>969</v>
@@ -52135,8 +52140,8 @@
       <c r="G10" s="4">
         <v>10.008333333333301</v>
       </c>
-      <c r="H10" s="4">
-        <v>28.611000000000001</v>
+      <c r="H10">
+        <v>118.611</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>969</v>
@@ -52197,8 +52202,8 @@
       <c r="G11" s="4">
         <v>12.925000000000001</v>
       </c>
-      <c r="H11" s="4">
-        <v>28.611000000000001</v>
+      <c r="H11">
+        <v>118.611</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>969</v>
@@ -52259,8 +52264,8 @@
       <c r="G12" s="5">
         <v>5.7916670000000003</v>
       </c>
-      <c r="H12" s="4">
-        <v>31.722000000000001</v>
+      <c r="H12">
+        <v>121.72200000000001</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>969</v>
@@ -52441,8 +52446,8 @@
       <c r="G15" s="4">
         <v>8.7083333333333304</v>
       </c>
-      <c r="H15" s="4">
-        <v>37.722000000000001</v>
+      <c r="H15">
+        <v>127.72200000000001</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>969</v>
@@ -69996,9 +70001,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65599BFC-5B06-4EDE-87C3-57BB3CCD5BDB}">
   <dimension ref="A1:AH29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y15" sqref="Y15"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>

</xml_diff>

<commit_message>
overlap percentage; fall models
</commit_message>
<xml_diff>
--- a/RawMaterials/data/LocalAdaptionDataGathering.xlsx
+++ b/RawMaterials/data/LocalAdaptionDataGathering.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Documents\git\localadaptclim\RawMaterials\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8310D2F5-23EC-4A47-A0BF-29C12E07A882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26E34D4-3DBB-4A63-B6F2-7E61C925E6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="920" firstSheet="29" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="920" firstSheet="23" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="6" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6767" uniqueCount="1205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6734" uniqueCount="1206">
   <si>
     <t>ID1</t>
   </si>
@@ -5167,6 +5167,9 @@
   </si>
   <si>
     <t>facet_plots_distribution_overlap</t>
+  </si>
+  <si>
+    <t>percentage_distribution_overlap</t>
   </si>
 </sst>
 </file>
@@ -45404,10 +45407,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA3977A-6DD7-4C46-8407-D260F17042BC}">
-  <dimension ref="A1:V119"/>
+  <dimension ref="A1:V145"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q55" sqref="Q14:R55"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -45620,8 +45623,8 @@
       <c r="H14">
         <v>146.50899999999999</v>
       </c>
-      <c r="I14" t="s">
-        <v>969</v>
+      <c r="I14">
+        <v>297.00599999999997</v>
       </c>
       <c r="J14">
         <v>51.9</v>
@@ -45679,8 +45682,8 @@
       <c r="H15">
         <v>151.846</v>
       </c>
-      <c r="I15" t="s">
-        <v>969</v>
+      <c r="I15">
+        <v>298.03399999999999</v>
       </c>
       <c r="J15">
         <v>51.9</v>
@@ -45738,8 +45741,8 @@
       <c r="H16">
         <v>145.29599999999999</v>
       </c>
-      <c r="I16" t="s">
-        <v>969</v>
+      <c r="I16">
+        <v>293.8</v>
       </c>
       <c r="J16">
         <v>51.9</v>
@@ -45797,8 +45800,8 @@
       <c r="H17">
         <v>147.965</v>
       </c>
-      <c r="I17" t="s">
-        <v>969</v>
+      <c r="I17">
+        <v>293.98200000000003</v>
       </c>
       <c r="J17">
         <v>51.9</v>
@@ -45856,8 +45859,8 @@
       <c r="H18">
         <v>149.178</v>
       </c>
-      <c r="I18" t="s">
-        <v>969</v>
+      <c r="I18">
+        <v>294.76799999999997</v>
       </c>
       <c r="J18">
         <v>51.9</v>
@@ -45915,8 +45918,8 @@
       <c r="H19">
         <v>150.876</v>
       </c>
-      <c r="I19" t="s">
-        <v>969</v>
+      <c r="I19">
+        <v>296.76400000000001</v>
       </c>
       <c r="J19">
         <v>51.9</v>
@@ -45974,8 +45977,8 @@
       <c r="H20">
         <v>149.25899999999999</v>
       </c>
-      <c r="I20" t="s">
-        <v>969</v>
+      <c r="I20">
+        <v>296.03800000000001</v>
       </c>
       <c r="J20">
         <v>51.9</v>
@@ -46033,8 +46036,8 @@
       <c r="H21">
         <v>148.85400000000001</v>
       </c>
-      <c r="I21" t="s">
-        <v>969</v>
+      <c r="I21">
+        <v>304.38499999999999</v>
       </c>
       <c r="J21">
         <v>51.9</v>
@@ -46093,8 +46096,8 @@
       <c r="H22">
         <v>150.95699999999999</v>
       </c>
-      <c r="I22" t="s">
-        <v>969</v>
+      <c r="I22">
+        <v>299.48599999999999</v>
       </c>
       <c r="J22">
         <v>51.9</v>
@@ -46152,8 +46155,8 @@
       <c r="H23">
         <v>151.44200000000001</v>
       </c>
-      <c r="I23" t="s">
-        <v>969</v>
+      <c r="I23">
+        <v>299.00200000000001</v>
       </c>
       <c r="J23">
         <v>51.9</v>
@@ -46211,8 +46214,8 @@
       <c r="H24">
         <v>150.714</v>
       </c>
-      <c r="I24" t="s">
-        <v>969</v>
+      <c r="I24">
+        <v>298.27600000000001</v>
       </c>
       <c r="J24">
         <v>51.9</v>
@@ -46270,8 +46273,8 @@
       <c r="H25">
         <v>146.34800000000001</v>
       </c>
-      <c r="I25" t="s">
-        <v>969</v>
+      <c r="I25">
+        <v>292.40899999999999</v>
       </c>
       <c r="J25">
         <v>51.9</v>
@@ -46329,8 +46332,8 @@
       <c r="H26">
         <v>147.965</v>
       </c>
-      <c r="I26" t="s">
-        <v>969</v>
+      <c r="I26">
+        <v>297.12700000000001</v>
       </c>
       <c r="J26">
         <v>51.9</v>
@@ -46388,8 +46391,8 @@
       <c r="H27">
         <v>149.744</v>
       </c>
-      <c r="I27" t="s">
-        <v>969</v>
+      <c r="I27">
+        <v>297.12700000000001</v>
       </c>
       <c r="J27">
         <v>51.9</v>
@@ -46447,8 +46450,8 @@
       <c r="H28">
         <v>148.69300000000001</v>
       </c>
-      <c r="I28" t="s">
-        <v>969</v>
+      <c r="I28">
+        <v>298.15499999999997</v>
       </c>
       <c r="J28">
         <v>51.9</v>
@@ -46506,8 +46509,8 @@
       <c r="H29">
         <v>149.66300000000001</v>
       </c>
-      <c r="I29" t="s">
-        <v>969</v>
+      <c r="I29">
+        <v>296.27999999999997</v>
       </c>
       <c r="J29">
         <v>51.9</v>
@@ -46565,8 +46568,8 @@
       <c r="H30">
         <v>151.44200000000001</v>
       </c>
-      <c r="I30" t="s">
-        <v>969</v>
+      <c r="I30">
+        <v>291.01799999999997</v>
       </c>
       <c r="J30">
         <v>51.9</v>
@@ -46624,8 +46627,8 @@
       <c r="H31">
         <v>149.01599999999999</v>
       </c>
-      <c r="I31" t="s">
-        <v>969</v>
+      <c r="I31">
+        <v>295.25200000000001</v>
       </c>
       <c r="J31">
         <v>51.9</v>
@@ -46683,8 +46686,8 @@
       <c r="H32">
         <v>155</v>
       </c>
-      <c r="I32" t="s">
-        <v>969</v>
+      <c r="I32">
+        <v>297.30799999999999</v>
       </c>
       <c r="J32">
         <v>51.9</v>
@@ -46742,8 +46745,8 @@
       <c r="H33">
         <v>149.744</v>
       </c>
-      <c r="I33" t="s">
-        <v>969</v>
+      <c r="I33">
+        <v>298.33699999999999</v>
       </c>
       <c r="J33">
         <v>51.9</v>
@@ -46801,8 +46804,8 @@
       <c r="H34">
         <v>146.10499999999999</v>
       </c>
-      <c r="I34" t="s">
-        <v>969</v>
+      <c r="I34">
+        <v>298.63900000000001</v>
       </c>
       <c r="J34">
         <v>51.9</v>
@@ -46860,8 +46863,8 @@
       <c r="H35">
         <v>148.28800000000001</v>
       </c>
-      <c r="I35" t="s">
-        <v>969</v>
+      <c r="I35">
+        <v>300.09100000000001</v>
       </c>
       <c r="J35">
         <v>51.9</v>
@@ -46919,8 +46922,8 @@
       <c r="H36">
         <v>149.34</v>
       </c>
-      <c r="I36" t="s">
-        <v>969</v>
+      <c r="I36">
+        <v>300.69600000000003</v>
       </c>
       <c r="J36">
         <v>51.9</v>
@@ -46978,8 +46981,8 @@
       <c r="H37">
         <v>145.94300000000001</v>
       </c>
-      <c r="I37" t="s">
-        <v>969</v>
+      <c r="I37">
+        <v>298.94200000000001</v>
       </c>
       <c r="J37">
         <v>51.9</v>
@@ -47037,8 +47040,8 @@
       <c r="H38">
         <v>149.09700000000001</v>
       </c>
-      <c r="I38" t="s">
-        <v>969</v>
+      <c r="I38">
+        <v>299.48599999999999</v>
       </c>
       <c r="J38">
         <v>51.9</v>
@@ -47096,8 +47099,8 @@
       <c r="H39">
         <v>146.34800000000001</v>
       </c>
-      <c r="I39" t="s">
-        <v>969</v>
+      <c r="I39">
+        <v>298.57900000000001</v>
       </c>
       <c r="J39">
         <v>51.9</v>
@@ -47155,8 +47158,8 @@
       <c r="H40">
         <v>148.12700000000001</v>
       </c>
-      <c r="I40" t="s">
-        <v>969</v>
+      <c r="I40">
+        <v>304.99</v>
       </c>
       <c r="J40">
         <v>51.9</v>
@@ -47214,8 +47217,8 @@
       <c r="H41">
         <v>144.56899999999999</v>
       </c>
-      <c r="I41" t="s">
-        <v>969</v>
+      <c r="I41">
+        <v>302.32900000000001</v>
       </c>
       <c r="J41">
         <v>51.9</v>
@@ -47273,8 +47276,8 @@
       <c r="H42">
         <v>145.054</v>
       </c>
-      <c r="I42" t="s">
-        <v>969</v>
+      <c r="I42">
+        <v>301.60300000000001</v>
       </c>
       <c r="J42">
         <v>51.9</v>
@@ -47332,8 +47335,8 @@
       <c r="H43">
         <v>145.21600000000001</v>
       </c>
-      <c r="I43" t="s">
-        <v>969</v>
+      <c r="I43">
+        <v>302.93299999999999</v>
       </c>
       <c r="J43">
         <v>51.9</v>
@@ -47391,8 +47394,8 @@
       <c r="H44">
         <v>145.78200000000001</v>
       </c>
-      <c r="I44" t="s">
-        <v>969</v>
+      <c r="I44">
+        <v>303.05399999999997</v>
       </c>
       <c r="J44">
         <v>51.9</v>
@@ -47450,8 +47453,8 @@
       <c r="H45">
         <v>146.995</v>
       </c>
-      <c r="I45" t="s">
-        <v>969</v>
+      <c r="I45">
+        <v>301.3</v>
       </c>
       <c r="J45">
         <v>51.9</v>
@@ -47509,8 +47512,8 @@
       <c r="H46">
         <v>145.53899999999999</v>
       </c>
-      <c r="I46" t="s">
-        <v>969</v>
+      <c r="I46">
+        <v>307.04599999999999</v>
       </c>
       <c r="J46">
         <v>51.9</v>
@@ -47568,8 +47571,8 @@
       <c r="H47">
         <v>139.636</v>
       </c>
-      <c r="I47" t="s">
-        <v>969</v>
+      <c r="I47">
+        <v>305.65499999999997</v>
       </c>
       <c r="J47">
         <v>51.9</v>
@@ -47627,8 +47630,8 @@
       <c r="H48">
         <v>146.59</v>
       </c>
-      <c r="I48" t="s">
-        <v>969</v>
+      <c r="I48">
+        <v>303.29599999999999</v>
       </c>
       <c r="J48">
         <v>51.9</v>
@@ -47686,8 +47689,8 @@
       <c r="H49">
         <v>141.577</v>
       </c>
-      <c r="I49" t="s">
-        <v>969</v>
+      <c r="I49">
+        <v>301.3</v>
       </c>
       <c r="J49">
         <v>51.9</v>
@@ -47745,8 +47748,8 @@
       <c r="H50">
         <v>144.97300000000001</v>
       </c>
-      <c r="I50" t="s">
-        <v>969</v>
+      <c r="I50">
+        <v>303.90100000000001</v>
       </c>
       <c r="J50">
         <v>51.9</v>
@@ -47805,8 +47808,8 @@
       <c r="H51">
         <v>144.40700000000001</v>
       </c>
-      <c r="I51" t="s">
-        <v>969</v>
+      <c r="I51">
+        <v>304.26400000000001</v>
       </c>
       <c r="J51">
         <v>51.9</v>
@@ -47864,8 +47867,8 @@
       <c r="H52">
         <v>145.13499999999999</v>
       </c>
-      <c r="I52" t="s">
-        <v>969</v>
+      <c r="I52">
+        <v>299.90899999999999</v>
       </c>
       <c r="J52">
         <v>51.9</v>
@@ -47923,8 +47926,8 @@
       <c r="H53">
         <v>141.739</v>
       </c>
-      <c r="I53" t="s">
-        <v>969</v>
+      <c r="I53">
+        <v>300.69600000000003</v>
       </c>
       <c r="J53">
         <v>51.9</v>
@@ -47983,8 +47986,8 @@
       <c r="H54">
         <v>142.46600000000001</v>
       </c>
-      <c r="I54" t="s">
-        <v>969</v>
+      <c r="I54">
+        <v>302.99400000000003</v>
       </c>
       <c r="J54">
         <v>51.9</v>
@@ -48042,8 +48045,8 @@
       <c r="H55">
         <v>141.72499999999999</v>
       </c>
-      <c r="I55" t="s">
-        <v>969</v>
+      <c r="I55">
+        <v>303.65899999999999</v>
       </c>
       <c r="J55">
         <v>51.9</v>
@@ -48860,7 +48863,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.6">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A97" t="s">
         <v>784</v>
       </c>
@@ -48892,7 +48895,7 @@
         <v>149.744</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.6">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A98" t="s">
         <v>785</v>
       </c>
@@ -48924,7 +48927,7 @@
         <v>146.10499999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.6">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A99" t="s">
         <v>786</v>
       </c>
@@ -48956,7 +48959,7 @@
         <v>148.28800000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.6">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A100" t="s">
         <v>787</v>
       </c>
@@ -48988,7 +48991,7 @@
         <v>149.34</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.6">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A101" t="s">
         <v>788</v>
       </c>
@@ -49020,7 +49023,7 @@
         <v>145.94300000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.6">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A102" t="s">
         <v>789</v>
       </c>
@@ -49052,7 +49055,7 @@
         <v>149.09700000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.6">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A103" t="s">
         <v>790</v>
       </c>
@@ -49081,7 +49084,7 @@
         <v>146.34800000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.6">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A104" t="s">
         <v>791</v>
       </c>
@@ -49112,8 +49115,29 @@
       <c r="K104">
         <v>148.12700000000001</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M104">
+        <v>42</v>
+      </c>
+      <c r="N104">
+        <v>0</v>
+      </c>
+      <c r="O104">
+        <v>57</v>
+      </c>
+      <c r="P104">
+        <v>57</v>
+      </c>
+      <c r="Q104">
+        <v>57</v>
+      </c>
+      <c r="R104">
+        <v>57.661000000000001</v>
+      </c>
+      <c r="S104">
+        <v>297.00599999999997</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A105" t="s">
         <v>792</v>
       </c>
@@ -49144,8 +49168,29 @@
       <c r="K105">
         <v>144.56899999999999</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M105">
+        <v>41</v>
+      </c>
+      <c r="N105">
+        <v>0</v>
+      </c>
+      <c r="O105">
+        <v>57</v>
+      </c>
+      <c r="P105">
+        <v>57</v>
+      </c>
+      <c r="Q105">
+        <v>57</v>
+      </c>
+      <c r="R105">
+        <v>57.587000000000003</v>
+      </c>
+      <c r="S105">
+        <v>298.03399999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A106" t="s">
         <v>794</v>
       </c>
@@ -49176,8 +49221,29 @@
       <c r="K106">
         <v>145.054</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M106">
+        <v>40</v>
+      </c>
+      <c r="N106">
+        <v>0</v>
+      </c>
+      <c r="O106">
+        <v>62</v>
+      </c>
+      <c r="P106">
+        <v>62</v>
+      </c>
+      <c r="Q106">
+        <v>62</v>
+      </c>
+      <c r="R106">
+        <v>57.523000000000003</v>
+      </c>
+      <c r="S106">
+        <v>293.8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A107" t="s">
         <v>795</v>
       </c>
@@ -49208,8 +49274,29 @@
       <c r="K107">
         <v>145.21600000000001</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M107">
+        <v>39</v>
+      </c>
+      <c r="N107">
+        <v>0</v>
+      </c>
+      <c r="O107">
+        <v>56</v>
+      </c>
+      <c r="P107">
+        <v>56</v>
+      </c>
+      <c r="Q107">
+        <v>56</v>
+      </c>
+      <c r="R107">
+        <v>57.302</v>
+      </c>
+      <c r="S107">
+        <v>293.98200000000003</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A108" t="s">
         <v>796</v>
       </c>
@@ -49240,8 +49327,29 @@
       <c r="K108">
         <v>145.78200000000001</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M108">
+        <v>38</v>
+      </c>
+      <c r="N108">
+        <v>0</v>
+      </c>
+      <c r="O108">
+        <v>59</v>
+      </c>
+      <c r="P108">
+        <v>59</v>
+      </c>
+      <c r="Q108">
+        <v>59</v>
+      </c>
+      <c r="R108">
+        <v>56.731999999999999</v>
+      </c>
+      <c r="S108">
+        <v>294.76799999999997</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A109" t="s">
         <v>797</v>
       </c>
@@ -49272,8 +49380,29 @@
       <c r="K109">
         <v>146.995</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M109">
+        <v>37</v>
+      </c>
+      <c r="N109">
+        <v>0</v>
+      </c>
+      <c r="O109">
+        <v>51</v>
+      </c>
+      <c r="P109">
+        <v>51</v>
+      </c>
+      <c r="Q109">
+        <v>51</v>
+      </c>
+      <c r="R109">
+        <v>56.720999999999997</v>
+      </c>
+      <c r="S109">
+        <v>296.76400000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A110" t="s">
         <v>798</v>
       </c>
@@ -49304,8 +49433,29 @@
       <c r="K110">
         <v>145.53899999999999</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M110">
+        <v>36</v>
+      </c>
+      <c r="N110">
+        <v>0</v>
+      </c>
+      <c r="O110">
+        <v>56</v>
+      </c>
+      <c r="P110">
+        <v>56</v>
+      </c>
+      <c r="Q110">
+        <v>56</v>
+      </c>
+      <c r="R110">
+        <v>56.667999999999999</v>
+      </c>
+      <c r="S110">
+        <v>296.03800000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A111" t="s">
         <v>799</v>
       </c>
@@ -49336,8 +49486,29 @@
       <c r="K111">
         <v>139.636</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M111">
+        <v>35</v>
+      </c>
+      <c r="N111">
+        <v>0</v>
+      </c>
+      <c r="O111">
+        <v>54</v>
+      </c>
+      <c r="P111">
+        <v>54</v>
+      </c>
+      <c r="Q111">
+        <v>54</v>
+      </c>
+      <c r="R111">
+        <v>56.646999999999998</v>
+      </c>
+      <c r="S111">
+        <v>304.38499999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A112" t="s">
         <v>800</v>
       </c>
@@ -49368,8 +49539,29 @@
       <c r="K112">
         <v>146.59</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M112">
+        <v>34</v>
+      </c>
+      <c r="N112">
+        <v>0</v>
+      </c>
+      <c r="O112">
+        <v>59</v>
+      </c>
+      <c r="P112">
+        <v>59</v>
+      </c>
+      <c r="Q112">
+        <v>59</v>
+      </c>
+      <c r="R112">
+        <v>56.658000000000001</v>
+      </c>
+      <c r="S112">
+        <v>299.48599999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A113" t="s">
         <v>801</v>
       </c>
@@ -49400,8 +49592,29 @@
       <c r="K113">
         <v>141.577</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M113">
+        <v>33</v>
+      </c>
+      <c r="N113">
+        <v>0</v>
+      </c>
+      <c r="O113">
+        <v>56</v>
+      </c>
+      <c r="P113">
+        <v>56</v>
+      </c>
+      <c r="Q113">
+        <v>56</v>
+      </c>
+      <c r="R113">
+        <v>56.625999999999998</v>
+      </c>
+      <c r="S113">
+        <v>299.00200000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A114" t="s">
         <v>802</v>
       </c>
@@ -49432,8 +49645,29 @@
       <c r="K114">
         <v>144.97300000000001</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M114">
+        <v>32</v>
+      </c>
+      <c r="N114">
+        <v>0</v>
+      </c>
+      <c r="O114">
+        <v>61</v>
+      </c>
+      <c r="P114">
+        <v>61</v>
+      </c>
+      <c r="Q114">
+        <v>61</v>
+      </c>
+      <c r="R114">
+        <v>56.351999999999997</v>
+      </c>
+      <c r="S114">
+        <v>298.27600000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A115" t="s">
         <v>803</v>
       </c>
@@ -49464,8 +49698,29 @@
       <c r="K115">
         <v>144.40700000000001</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M115">
+        <v>31</v>
+      </c>
+      <c r="N115">
+        <v>0</v>
+      </c>
+      <c r="O115">
+        <v>55</v>
+      </c>
+      <c r="P115">
+        <v>55</v>
+      </c>
+      <c r="Q115">
+        <v>55</v>
+      </c>
+      <c r="R115">
+        <v>56.151000000000003</v>
+      </c>
+      <c r="S115">
+        <v>292.40899999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A116" t="s">
         <v>804</v>
       </c>
@@ -49496,8 +49751,29 @@
       <c r="K116">
         <v>145.13499999999999</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M116">
+        <v>30</v>
+      </c>
+      <c r="N116">
+        <v>0</v>
+      </c>
+      <c r="O116">
+        <v>54</v>
+      </c>
+      <c r="P116">
+        <v>54</v>
+      </c>
+      <c r="Q116">
+        <v>54</v>
+      </c>
+      <c r="R116">
+        <v>55.960999999999999</v>
+      </c>
+      <c r="S116">
+        <v>297.12700000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A117" t="s">
         <v>805</v>
       </c>
@@ -49528,8 +49804,29 @@
       <c r="K117">
         <v>141.739</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M117">
+        <v>29</v>
+      </c>
+      <c r="N117">
+        <v>0</v>
+      </c>
+      <c r="O117">
+        <v>66</v>
+      </c>
+      <c r="P117">
+        <v>66</v>
+      </c>
+      <c r="Q117">
+        <v>66</v>
+      </c>
+      <c r="R117">
+        <v>55.761000000000003</v>
+      </c>
+      <c r="S117">
+        <v>297.12700000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A118" t="s">
         <v>806</v>
       </c>
@@ -49560,8 +49857,29 @@
       <c r="K118">
         <v>142.46600000000001</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="M118">
+        <v>28</v>
+      </c>
+      <c r="N118">
+        <v>0</v>
+      </c>
+      <c r="O118">
+        <v>59</v>
+      </c>
+      <c r="P118">
+        <v>59</v>
+      </c>
+      <c r="Q118">
+        <v>59</v>
+      </c>
+      <c r="R118">
+        <v>55.613</v>
+      </c>
+      <c r="S118">
+        <v>298.15499999999997</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.6">
       <c r="A119" t="s">
         <v>807</v>
       </c>
@@ -49592,8 +49910,630 @@
       <c r="K119">
         <v>141.72499999999999</v>
       </c>
+      <c r="M119">
+        <v>27</v>
+      </c>
+      <c r="N119">
+        <v>0</v>
+      </c>
+      <c r="O119">
+        <v>60</v>
+      </c>
+      <c r="P119">
+        <v>60</v>
+      </c>
+      <c r="Q119">
+        <v>60</v>
+      </c>
+      <c r="R119">
+        <v>55.381</v>
+      </c>
+      <c r="S119">
+        <v>296.27999999999997</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.6">
+      <c r="M120">
+        <v>26</v>
+      </c>
+      <c r="N120">
+        <v>0</v>
+      </c>
+      <c r="O120">
+        <v>57</v>
+      </c>
+      <c r="P120">
+        <v>57</v>
+      </c>
+      <c r="Q120">
+        <v>57</v>
+      </c>
+      <c r="R120">
+        <v>55.338999999999999</v>
+      </c>
+      <c r="S120">
+        <v>291.01799999999997</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.6">
+      <c r="M121">
+        <v>25</v>
+      </c>
+      <c r="N121">
+        <v>0</v>
+      </c>
+      <c r="O121">
+        <v>60</v>
+      </c>
+      <c r="P121">
+        <v>60</v>
+      </c>
+      <c r="Q121">
+        <v>60</v>
+      </c>
+      <c r="R121">
+        <v>55.222999999999999</v>
+      </c>
+      <c r="S121">
+        <v>295.25200000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.6">
+      <c r="M122">
+        <v>24</v>
+      </c>
+      <c r="N122">
+        <v>0</v>
+      </c>
+      <c r="O122">
+        <v>52</v>
+      </c>
+      <c r="P122">
+        <v>52</v>
+      </c>
+      <c r="Q122">
+        <v>52</v>
+      </c>
+      <c r="R122">
+        <v>55.095999999999997</v>
+      </c>
+      <c r="S122">
+        <v>297.30799999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.6">
+      <c r="M123">
+        <v>23</v>
+      </c>
+      <c r="N123">
+        <v>0</v>
+      </c>
+      <c r="O123">
+        <v>56</v>
+      </c>
+      <c r="P123">
+        <v>56</v>
+      </c>
+      <c r="Q123">
+        <v>56</v>
+      </c>
+      <c r="R123">
+        <v>54.747999999999998</v>
+      </c>
+      <c r="S123">
+        <v>298.33699999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.6">
+      <c r="M124">
+        <v>22</v>
+      </c>
+      <c r="N124">
+        <v>0</v>
+      </c>
+      <c r="O124">
+        <v>60</v>
+      </c>
+      <c r="P124">
+        <v>60</v>
+      </c>
+      <c r="Q124">
+        <v>60</v>
+      </c>
+      <c r="R124">
+        <v>54.241</v>
+      </c>
+      <c r="S124">
+        <v>298.63900000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.6">
+      <c r="M125">
+        <v>21</v>
+      </c>
+      <c r="N125">
+        <v>0</v>
+      </c>
+      <c r="O125">
+        <v>49</v>
+      </c>
+      <c r="P125">
+        <v>49</v>
+      </c>
+      <c r="Q125">
+        <v>49</v>
+      </c>
+      <c r="R125">
+        <v>54.23</v>
+      </c>
+      <c r="S125">
+        <v>300.09100000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.6">
+      <c r="M126">
+        <v>20</v>
+      </c>
+      <c r="N126">
+        <v>0</v>
+      </c>
+      <c r="O126">
+        <v>56</v>
+      </c>
+      <c r="P126">
+        <v>56</v>
+      </c>
+      <c r="Q126">
+        <v>56</v>
+      </c>
+      <c r="R126">
+        <v>54.23</v>
+      </c>
+      <c r="S126">
+        <v>300.69600000000003</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.6">
+      <c r="M127">
+        <v>19</v>
+      </c>
+      <c r="N127">
+        <v>0</v>
+      </c>
+      <c r="O127">
+        <v>53</v>
+      </c>
+      <c r="P127">
+        <v>53</v>
+      </c>
+      <c r="Q127">
+        <v>53</v>
+      </c>
+      <c r="R127">
+        <v>54.125</v>
+      </c>
+      <c r="S127">
+        <v>298.94200000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.6">
+      <c r="M128">
+        <v>18</v>
+      </c>
+      <c r="N128">
+        <v>0</v>
+      </c>
+      <c r="O128">
+        <v>63</v>
+      </c>
+      <c r="P128">
+        <v>63</v>
+      </c>
+      <c r="Q128">
+        <v>63</v>
+      </c>
+      <c r="R128">
+        <v>54.103999999999999</v>
+      </c>
+      <c r="S128">
+        <v>299.48599999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M129">
+        <v>17</v>
+      </c>
+      <c r="N129">
+        <v>0</v>
+      </c>
+      <c r="O129">
+        <v>56</v>
+      </c>
+      <c r="P129">
+        <v>56</v>
+      </c>
+      <c r="Q129">
+        <v>56</v>
+      </c>
+      <c r="R129">
+        <v>53.186</v>
+      </c>
+      <c r="S129">
+        <v>298.57900000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M130">
+        <v>16</v>
+      </c>
+      <c r="N130">
+        <v>0</v>
+      </c>
+      <c r="O130">
+        <v>55</v>
+      </c>
+      <c r="P130">
+        <v>55</v>
+      </c>
+      <c r="Q130">
+        <v>55</v>
+      </c>
+      <c r="R130">
+        <v>52.984999999999999</v>
+      </c>
+      <c r="S130">
+        <v>304.99</v>
+      </c>
+    </row>
+    <row r="131" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M131">
+        <v>15</v>
+      </c>
+      <c r="N131">
+        <v>0</v>
+      </c>
+      <c r="O131">
+        <v>58</v>
+      </c>
+      <c r="P131">
+        <v>58</v>
+      </c>
+      <c r="Q131">
+        <v>58</v>
+      </c>
+      <c r="R131">
+        <v>52.953000000000003</v>
+      </c>
+      <c r="S131">
+        <v>302.32900000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M132">
+        <v>14</v>
+      </c>
+      <c r="N132">
+        <v>0</v>
+      </c>
+      <c r="O132">
+        <v>57</v>
+      </c>
+      <c r="P132">
+        <v>57</v>
+      </c>
+      <c r="Q132">
+        <v>57</v>
+      </c>
+      <c r="R132">
+        <v>52.69</v>
+      </c>
+      <c r="S132">
+        <v>301.60300000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M133">
+        <v>13</v>
+      </c>
+      <c r="N133">
+        <v>0</v>
+      </c>
+      <c r="O133">
+        <v>48</v>
+      </c>
+      <c r="P133">
+        <v>48</v>
+      </c>
+      <c r="Q133">
+        <v>48</v>
+      </c>
+      <c r="R133">
+        <v>52.478000000000002</v>
+      </c>
+      <c r="S133">
+        <v>302.93299999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M134">
+        <v>12</v>
+      </c>
+      <c r="N134">
+        <v>0</v>
+      </c>
+      <c r="O134">
+        <v>51</v>
+      </c>
+      <c r="P134">
+        <v>51</v>
+      </c>
+      <c r="Q134">
+        <v>51</v>
+      </c>
+      <c r="R134">
+        <v>52.246000000000002</v>
+      </c>
+      <c r="S134">
+        <v>303.05399999999997</v>
+      </c>
+    </row>
+    <row r="135" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M135">
+        <v>11</v>
+      </c>
+      <c r="N135">
+        <v>0</v>
+      </c>
+      <c r="O135">
+        <v>56</v>
+      </c>
+      <c r="P135">
+        <v>56</v>
+      </c>
+      <c r="Q135">
+        <v>56</v>
+      </c>
+      <c r="R135">
+        <v>51.981999999999999</v>
+      </c>
+      <c r="S135">
+        <v>301.3</v>
+      </c>
+    </row>
+    <row r="136" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M136">
+        <v>10</v>
+      </c>
+      <c r="N136">
+        <v>0</v>
+      </c>
+      <c r="O136">
+        <v>56</v>
+      </c>
+      <c r="P136">
+        <v>56</v>
+      </c>
+      <c r="Q136">
+        <v>56</v>
+      </c>
+      <c r="R136">
+        <v>51.993000000000002</v>
+      </c>
+      <c r="S136">
+        <v>307.04599999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M137">
+        <v>9</v>
+      </c>
+      <c r="N137">
+        <v>0</v>
+      </c>
+      <c r="O137">
+        <v>57</v>
+      </c>
+      <c r="P137">
+        <v>57</v>
+      </c>
+      <c r="Q137">
+        <v>57</v>
+      </c>
+      <c r="R137">
+        <v>51.866</v>
+      </c>
+      <c r="S137">
+        <v>305.65499999999997</v>
+      </c>
+    </row>
+    <row r="138" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M138">
+        <v>8</v>
+      </c>
+      <c r="N138">
+        <v>0</v>
+      </c>
+      <c r="O138">
+        <v>56</v>
+      </c>
+      <c r="P138">
+        <v>56</v>
+      </c>
+      <c r="Q138">
+        <v>56</v>
+      </c>
+      <c r="R138">
+        <v>51.781999999999996</v>
+      </c>
+      <c r="S138">
+        <v>303.29599999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M139">
+        <v>7</v>
+      </c>
+      <c r="N139">
+        <v>0</v>
+      </c>
+      <c r="O139">
+        <v>56</v>
+      </c>
+      <c r="P139">
+        <v>56</v>
+      </c>
+      <c r="Q139">
+        <v>56</v>
+      </c>
+      <c r="R139">
+        <v>51.475999999999999</v>
+      </c>
+      <c r="S139">
+        <v>301.3</v>
+      </c>
+    </row>
+    <row r="140" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M140">
+        <v>6</v>
+      </c>
+      <c r="N140">
+        <v>0</v>
+      </c>
+      <c r="O140">
+        <v>56</v>
+      </c>
+      <c r="P140">
+        <v>56</v>
+      </c>
+      <c r="Q140">
+        <v>56</v>
+      </c>
+      <c r="R140">
+        <v>51.381</v>
+      </c>
+      <c r="S140">
+        <v>303.90100000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M141">
+        <v>5</v>
+      </c>
+      <c r="N141">
+        <v>0</v>
+      </c>
+      <c r="O141">
+        <v>57</v>
+      </c>
+      <c r="P141">
+        <v>57</v>
+      </c>
+      <c r="Q141">
+        <v>57</v>
+      </c>
+      <c r="R141">
+        <v>51.307000000000002</v>
+      </c>
+      <c r="S141">
+        <v>304.26400000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M142">
+        <v>4</v>
+      </c>
+      <c r="N142">
+        <v>0</v>
+      </c>
+      <c r="O142">
+        <v>62</v>
+      </c>
+      <c r="P142">
+        <v>62</v>
+      </c>
+      <c r="Q142">
+        <v>62</v>
+      </c>
+      <c r="R142">
+        <v>50.938000000000002</v>
+      </c>
+      <c r="S142">
+        <v>299.90899999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M143">
+        <v>3</v>
+      </c>
+      <c r="N143">
+        <v>0</v>
+      </c>
+      <c r="O143">
+        <v>56</v>
+      </c>
+      <c r="P143">
+        <v>56</v>
+      </c>
+      <c r="Q143">
+        <v>56</v>
+      </c>
+      <c r="R143">
+        <v>50.737000000000002</v>
+      </c>
+      <c r="S143">
+        <v>300.69600000000003</v>
+      </c>
+    </row>
+    <row r="144" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M144">
+        <v>2</v>
+      </c>
+      <c r="N144">
+        <v>0</v>
+      </c>
+      <c r="O144">
+        <v>55</v>
+      </c>
+      <c r="P144">
+        <v>55</v>
+      </c>
+      <c r="Q144">
+        <v>55</v>
+      </c>
+      <c r="R144">
+        <v>50.662999999999997</v>
+      </c>
+      <c r="S144">
+        <v>302.99400000000003</v>
+      </c>
+    </row>
+    <row r="145" spans="13:19" x14ac:dyDescent="0.6">
+      <c r="M145">
+        <v>1</v>
+      </c>
+      <c r="N145">
+        <v>0</v>
+      </c>
+      <c r="O145">
+        <v>57</v>
+      </c>
+      <c r="P145">
+        <v>57</v>
+      </c>
+      <c r="Q145">
+        <v>57</v>
+      </c>
+      <c r="R145">
+        <v>50.347000000000001</v>
+      </c>
+      <c r="S145">
+        <v>303.65899999999999</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M104:S145">
+    <sortCondition descending="1" ref="M104:M145"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -49602,8 +50542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2087B127-488B-4040-8438-14EA97B0549B}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q9:R24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -49725,8 +50665,8 @@
       <c r="H9">
         <v>116.96</v>
       </c>
-      <c r="I9" t="s">
-        <v>969</v>
+      <c r="I9">
+        <v>302.94</v>
       </c>
       <c r="J9" s="5">
         <v>42.957500000000003</v>
@@ -49784,8 +50724,8 @@
       <c r="H10">
         <v>115.01</v>
       </c>
-      <c r="I10" t="s">
-        <v>969</v>
+      <c r="I10">
+        <v>302.64400000000001</v>
       </c>
       <c r="J10" s="5">
         <v>42.957500000000003</v>
@@ -49844,8 +50784,8 @@
       <c r="H11">
         <v>115.62</v>
       </c>
-      <c r="I11" t="s">
-        <v>969</v>
+      <c r="I11">
+        <v>303.08800000000002</v>
       </c>
       <c r="J11" s="5">
         <v>42.957500000000003</v>
@@ -49904,8 +50844,8 @@
       <c r="H12">
         <v>116.96</v>
       </c>
-      <c r="I12" t="s">
-        <v>969</v>
+      <c r="I12">
+        <v>303.72899999999998</v>
       </c>
       <c r="J12" s="5">
         <v>42.957500000000003</v>
@@ -49964,8 +50904,8 @@
       <c r="H13">
         <v>117.36</v>
       </c>
-      <c r="I13" t="s">
-        <v>969</v>
+      <c r="I13">
+        <v>305.30700000000002</v>
       </c>
       <c r="J13" s="5">
         <v>42.957500000000003</v>
@@ -50024,8 +50964,8 @@
       <c r="H14">
         <v>115.62</v>
       </c>
-      <c r="I14" t="s">
-        <v>969</v>
+      <c r="I14">
+        <v>296.72699999999998</v>
       </c>
       <c r="J14" s="5">
         <v>42.957500000000003</v>
@@ -50084,8 +51024,8 @@
       <c r="H15">
         <v>113.63</v>
       </c>
-      <c r="I15" t="s">
-        <v>969</v>
+      <c r="I15">
+        <v>298.69900000000001</v>
       </c>
       <c r="J15" s="5">
         <v>42.957500000000003</v>
@@ -50144,8 +51084,8 @@
       <c r="H16">
         <v>114.35</v>
       </c>
-      <c r="I16" t="s">
-        <v>969</v>
+      <c r="I16">
+        <v>306.68799999999999</v>
       </c>
       <c r="J16" s="5">
         <v>42.957500000000003</v>
@@ -50204,8 +51144,8 @@
       <c r="H17">
         <v>107.93</v>
       </c>
-      <c r="I17" t="s">
-        <v>969</v>
+      <c r="I17">
+        <v>307.41500000000002</v>
       </c>
       <c r="J17" s="5">
         <v>42.957500000000003</v>
@@ -50264,8 +51204,8 @@
       <c r="H18">
         <v>105.11</v>
       </c>
-      <c r="I18" t="s">
-        <v>969</v>
+      <c r="I18">
+        <v>309.97399999999999</v>
       </c>
       <c r="J18" s="5">
         <v>42.957500000000003</v>
@@ -50324,8 +51264,8 @@
       <c r="H19">
         <v>105.88</v>
       </c>
-      <c r="I19" t="s">
-        <v>969</v>
+      <c r="I19">
+        <v>311.971</v>
       </c>
       <c r="J19" s="5">
         <v>42.957500000000003</v>
@@ -50384,8 +51324,8 @@
       <c r="H20">
         <v>108.18</v>
       </c>
-      <c r="I20" t="s">
-        <v>969</v>
+      <c r="I20">
+        <v>310.38400000000001</v>
       </c>
       <c r="J20" s="5">
         <v>42.957500000000003</v>
@@ -50444,8 +51384,8 @@
       <c r="H21">
         <v>107.16</v>
       </c>
-      <c r="I21" t="s">
-        <v>969</v>
+      <c r="I21">
+        <v>310.74200000000002</v>
       </c>
       <c r="J21" s="5">
         <v>42.957500000000003</v>
@@ -50504,8 +51444,8 @@
       <c r="H22">
         <v>105.75</v>
       </c>
-      <c r="I22" t="s">
-        <v>969</v>
+      <c r="I22">
+        <v>309.71800000000002</v>
       </c>
       <c r="J22" s="5">
         <v>42.957500000000003</v>
@@ -50564,8 +51504,8 @@
       <c r="H23">
         <v>101.15</v>
       </c>
-      <c r="I23" t="s">
-        <v>969</v>
+      <c r="I23">
+        <v>307.97800000000001</v>
       </c>
       <c r="J23" s="5">
         <v>42.957500000000003</v>
@@ -50624,8 +51564,8 @@
       <c r="H24">
         <v>103.83</v>
       </c>
-      <c r="I24" t="s">
-        <v>969</v>
+      <c r="I24">
+        <v>309.411</v>
       </c>
       <c r="J24" s="5">
         <v>42.957500000000003</v>
@@ -51928,7 +52868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4ECFFA-8AC8-4048-AA07-B0D2503C1E8B}">
   <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -61055,8 +61995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE38D98-9064-4846-BB7F-8B771A284B01}">
   <dimension ref="A1:T114"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D114"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -69999,11 +70939,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65599BFC-5B06-4EDE-87C3-57BB3CCD5BDB}">
-  <dimension ref="A1:AH29"/>
+  <dimension ref="A1:AI29"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B18" sqref="B18"/>
+      <pane xSplit="2" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -70018,10 +70958,10 @@
     <col min="9" max="9" width="18.09765625" customWidth="1"/>
     <col min="11" max="11" width="21.046875" customWidth="1"/>
     <col min="19" max="19" width="15.6484375" customWidth="1"/>
-    <col min="20" max="25" width="22.796875" customWidth="1"/>
+    <col min="20" max="26" width="22.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.6">
       <c r="B1" s="1" t="s">
         <v>652</v>
       </c>
@@ -70094,11 +71034,14 @@
       <c r="Y1" s="1" t="s">
         <v>1204</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="AA1" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -70171,8 +71114,11 @@
       <c r="X2" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.6">
+      <c r="Z2" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -70241,8 +71187,11 @@
         <v>672</v>
       </c>
       <c r="Y3" s="4"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.6">
+      <c r="Z3" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A19" si="0">A3+1</f>
         <v>3</v>
@@ -70311,18 +71260,21 @@
         <v>672</v>
       </c>
       <c r="Y4" s="10"/>
-      <c r="Z4" s="46" t="s">
+      <c r="Z4" t="s">
+        <v>672</v>
+      </c>
+      <c r="AA4" s="46" t="s">
         <v>685</v>
       </c>
-      <c r="AA4" s="46"/>
-      <c r="AC4" t="s">
+      <c r="AB4" s="46"/>
+      <c r="AD4" t="s">
         <v>991</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>1114</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -70370,14 +71322,14 @@
       <c r="U5" t="s">
         <v>695</v>
       </c>
-      <c r="Z5" s="61" t="s">
+      <c r="AA5" s="61" t="s">
         <v>697</v>
       </c>
-      <c r="AA5" s="61"/>
       <c r="AB5" s="61"/>
       <c r="AC5" s="61"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.6">
+      <c r="AD5" s="61"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -70445,8 +71397,11 @@
       <c r="X6" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.6">
+      <c r="Z6" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -70511,8 +71466,11 @@
       <c r="X7" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.6">
+      <c r="Z7" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -70577,8 +71535,11 @@
       <c r="X8" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.6">
+      <c r="Z8" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -70647,10 +71608,13 @@
         <v>672</v>
       </c>
       <c r="Z9" t="s">
+        <v>672</v>
+      </c>
+      <c r="AA9" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -70719,10 +71683,13 @@
         <v>672</v>
       </c>
       <c r="Z10" t="s">
+        <v>672</v>
+      </c>
+      <c r="AA10" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -70792,17 +71759,18 @@
       </c>
       <c r="X11" s="63"/>
       <c r="Y11" s="63"/>
-      <c r="Z11" t="s">
+      <c r="Z11" s="63"/>
+      <c r="AA11" t="s">
         <v>731</v>
       </c>
-      <c r="AG11" s="1" t="s">
+      <c r="AH11" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AI11" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -70868,16 +71836,19 @@
         <v>672</v>
       </c>
       <c r="Z12" t="s">
+        <v>672</v>
+      </c>
+      <c r="AA12" t="s">
         <v>732</v>
       </c>
-      <c r="AG12" s="1" t="s">
+      <c r="AH12" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AI12" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -70940,16 +71911,19 @@
         <v>672</v>
       </c>
       <c r="Z13" t="s">
+        <v>672</v>
+      </c>
+      <c r="AA13" t="s">
         <v>622</v>
       </c>
-      <c r="AG13" s="1" t="s">
+      <c r="AH13" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="AH13" t="s">
+      <c r="AI13" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -71017,14 +71991,17 @@
       <c r="Y14" t="s">
         <v>672</v>
       </c>
-      <c r="AG14" s="1" t="s">
+      <c r="Z14" t="s">
+        <v>672</v>
+      </c>
+      <c r="AH14" s="1" t="s">
         <v>637</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AI14" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -71068,17 +72045,17 @@
       <c r="U15" s="62" t="s">
         <v>672</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
         <v>887</v>
       </c>
-      <c r="AG15" s="1" t="s">
+      <c r="AH15" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="AH15" t="s">
+      <c r="AI15" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -71146,14 +72123,17 @@
       <c r="Y16" t="s">
         <v>672</v>
       </c>
-      <c r="AG16" s="1" t="s">
+      <c r="Z16" t="s">
+        <v>672</v>
+      </c>
+      <c r="AH16" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="AH16" t="s">
+      <c r="AI16" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -71218,14 +72198,17 @@
       <c r="X17" t="s">
         <v>672</v>
       </c>
-      <c r="AG17" s="1" t="s">
+      <c r="Z17" t="s">
+        <v>672</v>
+      </c>
+      <c r="AH17" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="AH17" t="s">
+      <c r="AI17" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -71290,23 +72273,26 @@
       <c r="X18" t="s">
         <v>672</v>
       </c>
-      <c r="Z18" s="63" t="s">
+      <c r="Z18" t="s">
+        <v>672</v>
+      </c>
+      <c r="AA18" s="63" t="s">
         <v>1200</v>
       </c>
-      <c r="AA18" s="63"/>
       <c r="AB18" s="63"/>
       <c r="AC18" s="63"/>
       <c r="AD18" s="63"/>
       <c r="AE18" s="63"/>
       <c r="AF18" s="63"/>
-      <c r="AG18" s="1" t="s">
+      <c r="AG18" s="63"/>
+      <c r="AH18" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="AH18" t="s">
+      <c r="AI18" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -71374,14 +72360,17 @@
       <c r="X19" t="s">
         <v>672</v>
       </c>
-      <c r="AG19" s="1" t="s">
+      <c r="Z19" t="s">
+        <v>672</v>
+      </c>
+      <c r="AH19" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="AH19" t="s">
+      <c r="AI19" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A20">
         <v>19</v>
       </c>
@@ -71448,14 +72437,17 @@
       <c r="X20" t="s">
         <v>672</v>
       </c>
-      <c r="AG20" s="1" t="s">
+      <c r="Z20" t="s">
+        <v>672</v>
+      </c>
+      <c r="AH20" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="AH20" t="s">
+      <c r="AI20" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A21">
         <f>A20+1</f>
         <v>20</v>
@@ -71523,14 +72515,17 @@
       <c r="X21" t="s">
         <v>672</v>
       </c>
-      <c r="AG21" s="1" t="s">
+      <c r="Z21" t="s">
+        <v>672</v>
+      </c>
+      <c r="AH21" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="AH21" t="s">
+      <c r="AI21" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A22">
         <f t="shared" ref="A22:A26" si="1">A21+1</f>
         <v>21</v>
@@ -71598,14 +72593,17 @@
       <c r="X22" t="s">
         <v>672</v>
       </c>
-      <c r="AG22" s="1" t="s">
+      <c r="Z22" t="s">
+        <v>672</v>
+      </c>
+      <c r="AH22" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="AH22" t="s">
+      <c r="AI22" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -71649,15 +72647,32 @@
       <c r="N23" t="s">
         <v>672</v>
       </c>
-      <c r="R23" s="17"/>
-      <c r="AG23" s="1" t="s">
+      <c r="P23" t="s">
+        <v>672</v>
+      </c>
+      <c r="R23" t="s">
+        <v>672</v>
+      </c>
+      <c r="S23" t="s">
+        <v>672</v>
+      </c>
+      <c r="T23" t="s">
+        <v>672</v>
+      </c>
+      <c r="W23" t="s">
+        <v>695</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>672</v>
+      </c>
+      <c r="AH23" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="AH23" t="s">
+      <c r="AI23" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -71696,14 +72711,14 @@
       <c r="M24" s="15" t="s">
         <v>1148</v>
       </c>
-      <c r="AG24" s="1" t="s">
+      <c r="AH24" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="AH24" t="s">
+      <c r="AI24" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -71729,14 +72744,14 @@
       <c r="N25" t="s">
         <v>1155</v>
       </c>
-      <c r="AG25" s="1" t="s">
+      <c r="AH25" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="AH25" t="s">
+      <c r="AI25" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.6">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -71780,14 +72795,14 @@
       <c r="N26" t="s">
         <v>1179</v>
       </c>
-      <c r="AG26" s="1" t="s">
+      <c r="AH26" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="AH26" t="s">
+      <c r="AI26" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.6">
       <c r="B27" s="52" t="s">
         <v>1180</v>
       </c>
@@ -71822,7 +72837,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.6">
       <c r="B28" s="10" t="s">
         <v>1187</v>
       </c>
@@ -71860,7 +72875,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.6">
       <c r="B29" s="10" t="s">
         <v>1188</v>
       </c>

</xml_diff>

<commit_message>
sync progress to git
</commit_message>
<xml_diff>
--- a/RawMaterials/data/LocalAdaptionDataGathering.xlsx
+++ b/RawMaterials/data/LocalAdaptionDataGathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Documents\git\localadaptclim\RawMaterials\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEDFC26-5750-4392-A74F-9E2296C0C73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342C1A33-AEB1-491E-B368-AF843D0A4708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="920" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79915,9 +79915,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65599BFC-5B06-4EDE-87C3-57BB3CCD5BDB}">
   <dimension ref="A1:AJ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>

</xml_diff>